<commit_message>
Aakash and Madujith time sheet updation
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C38337B2-1877-4A3E-BE25-D932695121B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C6D3A6E-9009-444D-903E-2A72C2015867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="75">
   <si>
     <t>Resource Name</t>
   </si>
@@ -261,12 +261,52 @@
     <t>1-2-2-1</t>
   </si>
   <si>
+    <t>Redesigning the home page, Dashboard in Admin page</t>
+  </si>
+  <si>
+    <t>1)Designed Wireframe for the Public and Approver pages
+2)Discussion about redesigning the wireframe 
+3)Session about design pattern (abstract factory)</t>
+  </si>
+  <si>
+    <t>Wire framing for the UI of HR page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4
+1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+-
+2
+</t>
+  </si>
+  <si>
     <t>1.Acceptance criteria 
 2.Dependencies 
 3.Assumptions</t>
   </si>
   <si>
     <t>1.Discussion on prototype.                                            2.Reworking on wire frame for  the Requester (Award page,my request page)and Approver(Award page,my request page,approver page)</t>
+  </si>
+  <si>
+    <t>Redesinging the Home page wireframe</t>
+  </si>
+  <si>
+    <t>1).Designed  homepage  wireframe. 2)Explored about Prototype design pattern.3)Disscussion meeting about  redesigning the wireframe 4) Dessign pattern session( abstract factory)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3
+-
+1
+</t>
+  </si>
+  <si>
+    <t>-
+2
+-
+1</t>
   </si>
 </sst>
 </file>
@@ -1288,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE42D53-7E04-4254-8D5E-88A8C21EAC94}">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H12"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.25" customHeight="1"/>
@@ -1736,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8350AC00-EFFB-42E3-B11C-77314475CC20}">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1858,24 +1898,24 @@
       </c>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="2:8" ht="229.5">
+    <row r="7" spans="2:8" ht="101.25" customHeight="1">
       <c r="B7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="H7" s="31"/>
     </row>
@@ -1884,7 +1924,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>62</v>
@@ -1905,7 +1945,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>59</v>
@@ -1921,7 +1961,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="2:8" ht="204">
+    <row r="10" spans="2:8" ht="63.75">
       <c r="B10" s="17" t="s">
         <v>29</v>
       </c>
@@ -1942,37 +1982,35 @@
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="2:8" ht="204">
+    <row r="11" spans="2:8" ht="76.5">
       <c r="B11" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="2:8" ht="191.25">
+    <row r="12" spans="2:8" ht="25.5">
       <c r="B12" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="D12" s="13"/>
       <c r="E12" s="27" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Madujith time sheet updation
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF9D9844-FE05-4AE4-8DCD-83B6A181F316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA8CC3E8-FDA9-47C1-A208-FF30F99FA14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05-04-2022" sheetId="40" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="102">
   <si>
     <t>Resource Name</t>
   </si>
@@ -356,6 +356,14 @@
 3. Session on Design Pattern - Builder, Prototype
 4. Meeting with Rafi(MOM)
 5. Discussion About the Meeting with Team.</t>
+  </si>
+  <si>
+    <t>1.Reworked on Wireframe for Admin(Manage employee,Manage Award,Manage Orz)
+2.Discussion About Meeting with Team
+3.Rechecked All Wireframes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.Meeting with rafi(wire frame)                                                  2.Session on DesignPattern - Builder,Prototype. 3.Rework on prototype(Admin)</t>
   </si>
   <si>
     <t>Improving the wireframe with neat flow</t>
@@ -2135,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141F7631-8030-4C9D-96AB-26E10E8B9306}">
   <dimension ref="B4:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2237,16 +2245,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="G8" s="33">
         <v>1</v>
@@ -2258,19 +2266,19 @@
         <v>12</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H9" s="31"/>
     </row>
@@ -2288,7 +2296,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G10" s="14">
         <v>1</v>
@@ -2300,10 +2308,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>24</v>
@@ -2342,19 +2350,19 @@
         <v>16</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H13" s="12"/>
     </row>
@@ -2363,16 +2371,16 @@
         <v>30</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="G14" s="28" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
AAkash and Madujith's timesheet
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FF7D287-0B31-49A8-94BF-19FA525C08D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A45B301-481B-4B40-B47E-354AE930B3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="115">
   <si>
     <t>Resource Name</t>
   </si>
@@ -459,6 +459,16 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>1)Brain Storming with team 
+2).Refining the Home page and landing page wireframes  3) discussion meeting about redesigning the wireframe and spliting the work between teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1
+4
+1
+</t>
   </si>
 </sst>
 </file>
@@ -2185,7 +2195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3A5E95-3FAF-42D8-986E-9C3B3ED96D50}">
   <dimension ref="B4:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2436,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141F7631-8030-4C9D-96AB-26E10E8B9306}">
   <dimension ref="B4:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2646,16 +2656,16 @@
         <v>109</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H13" s="12"/>
     </row>
@@ -2666,14 +2676,14 @@
       <c r="C14" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>89</v>
+      <c r="D14" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="G14" s="28" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Aravinth, Logesh - Updated Timesheet
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="463" documentId="8_{CF9D9844-FE05-4AE4-8DCD-83B6A181F316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAF51D1A-8401-4630-BB16-E337642E5B03}"/>
+  <xr:revisionPtr revIDLastSave="664" documentId="8_{CF9D9844-FE05-4AE4-8DCD-83B6A181F316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A4C3BC4-016B-4A5C-83FE-DB3CD90F65C8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05-04-2022" sheetId="40" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="09-04-2022 " sheetId="45" r:id="rId5"/>
     <sheet name="11-04-2022" sheetId="43" r:id="rId6"/>
     <sheet name="12-04-2022" sheetId="46" r:id="rId7"/>
+    <sheet name="13-04-2022" sheetId="47" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="214">
   <si>
     <t>Resource Name</t>
   </si>
@@ -646,12 +647,138 @@
   <si>
     <t xml:space="preserve">1 hour </t>
   </si>
+  <si>
+    <t>sample data for data model(excel sheet)</t>
+  </si>
+  <si>
+    <t>30mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wireframe for approver(changed naming conventions,Add request)</t>
+  </si>
+  <si>
+    <t>refined the user story</t>
+  </si>
+  <si>
+    <t>1hr30mins</t>
+  </si>
+  <si>
+    <t>College review</t>
+  </si>
+  <si>
+    <t>Meeting with Rafi( About Lesson,data model.physical model,view model )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hr </t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>Normalisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Data Model </t>
+  </si>
+  <si>
+    <t>2hr 30mins</t>
+  </si>
+  <si>
+    <t>Meeting with Rafi( plan for next 3days )</t>
+  </si>
+  <si>
+    <t>1hr</t>
+  </si>
+  <si>
+    <t>entering MOM For Last day</t>
+  </si>
+  <si>
+    <t>1/2 hr</t>
+  </si>
+  <si>
+    <t>Logo removed for all wireframe pages some alignment corrections</t>
+  </si>
+  <si>
+    <t>Session about lesson learned (planning for 4 days - Services, Operations, class diagram, view model)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refining Constraints, dependencies for each user story </t>
+  </si>
+  <si>
+    <t>2 hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               30mins</t>
+  </si>
+  <si>
+    <t>Normalization</t>
+  </si>
+  <si>
+    <t>1hr15mins</t>
+  </si>
+  <si>
+    <t>Dashboard modiications</t>
+  </si>
+  <si>
+    <t>Rechecked the Prototype with the last MOM - 1hr</t>
+  </si>
+  <si>
+    <t>3.5hrs</t>
+  </si>
+  <si>
+    <t>15mins</t>
+  </si>
+  <si>
+    <t>Discussed and implemented the Physical model - 1hrs</t>
+  </si>
+  <si>
+    <t>Project Review Preparation</t>
+  </si>
+  <si>
+    <t>Checked Admin flow</t>
+  </si>
+  <si>
+    <t>wireframe for requester(Add Request)</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>rechecked wireframe for approver(Add Request,changed naming conventions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wireframe for HR(Add Request)</t>
+  </si>
+  <si>
+    <t>1.15min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  rechecked wireframe for admin(refined flow for awards,employee,organisation,department)</t>
+  </si>
+  <si>
+    <t>Learned normalization concepts</t>
+  </si>
+  <si>
+    <t>Refining use cases(dependencies,constraints)</t>
+  </si>
+  <si>
+    <t>Session with Rafi about Lessions learned in project training and what to do for next 7 days</t>
+  </si>
+  <si>
+    <t>Session with Rafi regarding lessons learned and what we are going to do till next mid week</t>
+  </si>
+  <si>
+    <t>Refined the user story</t>
+  </si>
+  <si>
+    <t>Meeting with Rafi( About Lesson,data model,physical model,view model )</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -797,6 +924,21 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -811,7 +953,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -949,6 +1091,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -959,8 +1112,8 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
@@ -970,13 +1123,104 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -985,7 +1229,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1116,95 +1360,181 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3678,8 +4008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD40CF5-BD55-4D10-8C22-DF938ABB531A}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D10"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C50" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3691,616 +4021,585 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="72" t="s">
+      <c r="D2" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="52"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="60"/>
-      <c r="B3" s="46" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="70" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="54"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="60"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46" t="s">
+      <c r="A4" s="88"/>
+      <c r="C4" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="70" t="s">
+      <c r="D4" s="84"/>
+      <c r="E4" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="F4" s="70"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="49"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="74"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56" t="s">
+      <c r="A5" s="89"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="73" t="s">
+      <c r="D5" s="85"/>
+      <c r="E5" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="57"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="51"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" t="s">
         <v>135</v>
       </c>
       <c r="C6" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="83" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="54"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="49"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="61"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46" t="s">
+      <c r="A7" s="90"/>
+      <c r="C7" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="70" t="s">
+      <c r="D7" s="84"/>
+      <c r="E7" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="F7" s="70"/>
-      <c r="G7" s="54"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="49"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="61"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="54"/>
+      <c r="A8" s="90"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="61"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="54"/>
+      <c r="A9" s="90"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="49"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="61"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="70" t="s">
+      <c r="A10" s="91"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="54"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="49"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="72"/>
-      <c r="G11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="62"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46" t="s">
+      <c r="A12" s="92"/>
+      <c r="C12" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70" t="s">
+      <c r="D12" s="84"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="G12" s="54"/>
+      <c r="G12" s="49"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="62"/>
-      <c r="B13" s="46" t="s">
+      <c r="A13" s="92"/>
+      <c r="B13" t="s">
         <v>145</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="70" t="s">
+      <c r="D13" s="84"/>
+      <c r="E13" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="F13" s="70"/>
-      <c r="G13" s="54"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="62"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46" t="s">
+      <c r="A14" s="92"/>
+      <c r="C14" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="54"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="62"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="54"/>
+      <c r="A15" s="92"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="49"/>
     </row>
     <row r="16" spans="1:7" ht="21.75" customHeight="1">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="72" t="s">
+      <c r="D16" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="72"/>
-      <c r="G16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A17" s="80"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46" t="s">
+      <c r="A17" s="78"/>
+      <c r="C17" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="70">
+      <c r="D17" s="84"/>
+      <c r="E17" s="46">
         <v>1.5</v>
       </c>
-      <c r="F17" s="70"/>
-      <c r="G17" s="54"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A18" s="80"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46" t="s">
+      <c r="A18" s="78"/>
+      <c r="C18" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70">
+      <c r="D18" s="84"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46">
         <v>1.5</v>
       </c>
-      <c r="G18" s="54"/>
+      <c r="G18" s="49"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A19" s="81"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46" t="s">
+      <c r="A19" s="78"/>
+      <c r="C19" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="71">
+      <c r="D19" s="85"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="57">
         <v>0.5</v>
       </c>
-      <c r="G19" s="54"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="53"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46" t="s">
+      <c r="A21" s="78"/>
+      <c r="C21" t="s">
         <v>154</v>
       </c>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="54"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="49"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="55"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75" t="s">
+      <c r="A22" s="79"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="D22" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="77" t="s">
+      <c r="D22" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="78"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="51"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="70" t="s">
+      <c r="D23" s="83"/>
+      <c r="E23" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="70"/>
-      <c r="G23" s="54"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="80"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46" t="s">
+      <c r="A24" s="86"/>
+      <c r="C24" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="70">
+      <c r="D24" s="84"/>
+      <c r="E24" s="46">
         <v>2</v>
       </c>
-      <c r="F24" s="70"/>
-      <c r="G24" s="54"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="49"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="80"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46" t="s">
+      <c r="A25" s="86"/>
+      <c r="C25" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="49"/>
-      <c r="E25" s="47">
+      <c r="D25" s="84"/>
+      <c r="E25" s="46">
         <v>1</v>
       </c>
-      <c r="F25" s="70"/>
-      <c r="G25" s="54"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="81"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46" t="s">
+      <c r="A26" s="86"/>
+      <c r="C26" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="70">
+      <c r="D26" s="85"/>
+      <c r="E26" s="46">
         <v>1</v>
       </c>
-      <c r="F26" s="70"/>
-      <c r="G26" s="54"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="49"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="72" t="s">
+      <c r="D27" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="F27" s="72"/>
-      <c r="G27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="53"/>
+      <c r="A28" s="78"/>
       <c r="B28" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="70" t="s">
+      <c r="D28" s="84"/>
+      <c r="E28" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="70"/>
-      <c r="G28" s="54"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="49"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="53"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46" t="s">
+      <c r="A29" s="78"/>
+      <c r="C29" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="70" t="s">
+      <c r="D29" s="84"/>
+      <c r="E29" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="F29" s="70"/>
-      <c r="G29" s="54"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A30" s="55"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56" t="s">
+      <c r="A30" s="78"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="73" t="s">
+      <c r="D30" s="85"/>
+      <c r="E30" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="73"/>
-      <c r="G30" s="57"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="51"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="54"/>
+      <c r="D31" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="49"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="53"/>
-      <c r="B32" s="46" t="s">
+      <c r="A32" s="78"/>
+      <c r="B32" t="s">
         <v>161</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" t="s">
         <v>162</v>
       </c>
-      <c r="D32" s="68"/>
-      <c r="E32" s="70" t="s">
+      <c r="D32" s="81"/>
+      <c r="E32" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="F32" s="70"/>
-      <c r="G32" s="54"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="49"/>
     </row>
     <row r="33" spans="1:7" ht="21" customHeight="1">
-      <c r="A33" s="53"/>
-      <c r="B33" s="46" t="s">
+      <c r="A33" s="78"/>
+      <c r="B33" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="68"/>
-      <c r="E33" s="70" t="s">
+      <c r="D33" s="81"/>
+      <c r="E33" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="F33" s="70"/>
-      <c r="G33" s="54"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="49"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="53"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="54"/>
+      <c r="A34" s="78"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="49"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="53"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="54"/>
+      <c r="A35" s="78"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="49"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51" t="s">
+      <c r="B36" s="47"/>
+      <c r="C36" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="D36" s="59"/>
-      <c r="E36" s="72" t="s">
+      <c r="D36" s="83"/>
+      <c r="E36" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="F36" s="72"/>
-      <c r="G36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="53"/>
-      <c r="B37" s="46" t="s">
+      <c r="A37" s="78"/>
+      <c r="B37" t="s">
         <v>166</v>
       </c>
       <c r="C37" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="70" t="s">
+      <c r="D37" s="84"/>
+      <c r="E37" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="F37" s="70"/>
-      <c r="G37" s="54"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="49"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="53"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46" t="s">
+      <c r="A38" s="78"/>
+      <c r="C38" t="s">
         <v>169</v>
       </c>
-      <c r="D38" s="49"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70" t="s">
+      <c r="D38" s="84"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="G38" s="54"/>
+      <c r="G38" s="49"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="53"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="54"/>
+      <c r="A39" s="78"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="49"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="55"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="57"/>
+      <c r="A40" s="79"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="51"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="70"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="54"/>
+      <c r="D41" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="46"/>
+      <c r="G41" s="49"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="53"/>
-      <c r="B42" s="46"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="54"/>
+      <c r="A42" s="78"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="46"/>
+      <c r="G42" s="49"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="53"/>
-      <c r="B43" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="46" t="s">
+      <c r="A43" s="78"/>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" t="s">
         <v>162</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="70" t="s">
+      <c r="D43" s="84"/>
+      <c r="E43" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="F43" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="G43" s="54"/>
+      <c r="F43" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="49"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="53"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="54"/>
+      <c r="A44" s="78"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="46"/>
+      <c r="G44" s="49"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="55"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="57"/>
+      <c r="A45" s="79"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="51"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="D46" s="47"/>
+      <c r="D46" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="D2:D5"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="A41:A45"/>
     <mergeCell ref="D31:D35"/>
@@ -4313,13 +4612,726 @@
     <mergeCell ref="D41:D45"/>
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="A31:A35"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A15"/>
     <mergeCell ref="A27:A30"/>
-    <mergeCell ref="D2:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5078C7BA-40AD-44B2-B44A-F90FDEF2CC2F}">
+  <dimension ref="A1:G55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" customWidth="1"/>
+    <col min="3" max="3" width="94.7109375" customWidth="1"/>
+    <col min="4" max="7" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="59"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="98"/>
+      <c r="B3" s="66" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="101"/>
+      <c r="E3" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="63"/>
+      <c r="G3" s="60"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="98"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="101"/>
+      <c r="E4" s="57" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="63"/>
+      <c r="G4" s="60"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="98"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="101"/>
+      <c r="E5" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="63"/>
+      <c r="G5" s="60"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="98"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="101"/>
+      <c r="E6" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="63"/>
+      <c r="G6" s="60"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="99"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="102"/>
+      <c r="E7" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" s="64"/>
+      <c r="G7" s="61"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="103" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="95" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="103"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="95"/>
+      <c r="E9" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="103"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="95"/>
+      <c r="E10" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="104"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="95"/>
+      <c r="E11" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="94" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="103"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="95"/>
+      <c r="E13" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="103"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="95"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="60"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="103"/>
+      <c r="B15" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="57"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="104"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+    </row>
+    <row r="17" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A17" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="66"/>
+      <c r="C17" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A18" s="93"/>
+      <c r="B18" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="95"/>
+      <c r="E18" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A19" s="93"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" s="95"/>
+      <c r="E19" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+    </row>
+    <row r="20" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A20" s="93"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="95"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="G20" s="60"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="105" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="94" t="s">
+        <v>197</v>
+      </c>
+      <c r="F21" s="107" t="s">
+        <v>198</v>
+      </c>
+      <c r="G21" s="59"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="93"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="108"/>
+      <c r="G22" s="60"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="93"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="61"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="95"/>
+      <c r="E24" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="93"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" s="95"/>
+      <c r="E25" s="63">
+        <v>2</v>
+      </c>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="93"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66" t="s">
+        <v>181</v>
+      </c>
+      <c r="D26" s="95"/>
+      <c r="E26" s="63">
+        <v>1</v>
+      </c>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="106"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="D27" s="96"/>
+      <c r="E27" s="63">
+        <v>1</v>
+      </c>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="62" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="59"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="93"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="95"/>
+      <c r="E29" s="63" t="s">
+        <v>203</v>
+      </c>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="93"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" s="95"/>
+      <c r="E30" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="93"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="D31" s="95"/>
+      <c r="E31" s="63" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="93"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" s="95"/>
+      <c r="E32" s="63" t="s">
+        <v>206</v>
+      </c>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+    </row>
+    <row r="33" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A33" s="93"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="D33" s="96"/>
+      <c r="E33" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="105" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="63"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="93"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66" t="s">
+        <v>208</v>
+      </c>
+      <c r="D35" s="95"/>
+      <c r="E35" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+    </row>
+    <row r="36" spans="1:7" ht="21" customHeight="1">
+      <c r="A36" s="93"/>
+      <c r="B36" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="C36" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="95"/>
+      <c r="E36" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="93"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" s="95"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="60"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="93"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="94"/>
+      <c r="E39" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="93"/>
+      <c r="B40" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="95"/>
+      <c r="E40" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="93"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66" t="s">
+        <v>211</v>
+      </c>
+      <c r="D41" s="95"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="G41" s="60"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="93"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="106"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="61"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="66"/>
+      <c r="C44" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="F44" s="62"/>
+      <c r="G44" s="60"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="93"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="95"/>
+      <c r="E45" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="F45" s="63"/>
+      <c r="G45" s="60"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="93"/>
+      <c r="B46" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="66" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" s="95"/>
+      <c r="E46" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="F46" s="76"/>
+      <c r="G46" s="60"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="93"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="66" t="s">
+        <v>213</v>
+      </c>
+      <c r="D47" s="95"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="G47" s="60"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="106"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="61"/>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" s="46"/>
+    </row>
+    <row r="55" spans="4:5">
+      <c r="E55" s="75"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="D28:D33"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D21:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>